<commit_message>
add  client db testing
</commit_message>
<xml_diff>
--- a/Data/MyData.xlsx
+++ b/Data/MyData.xlsx
@@ -281,7 +281,7 @@
     <t>tax_code</t>
   </si>
   <si>
-    <t>AmolDB002</t>
+    <t>AmolDB006</t>
   </si>
 </sst>
 </file>
@@ -869,7 +869,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>